<commit_message>
changed graphic | databases
</commit_message>
<xml_diff>
--- a/2025/first_semester/usupova_n_m/databases/excel_tasks/plotting_13_1_4.xlsx
+++ b/2025/first_semester/usupova_n_m/databases/excel_tasks/plotting_13_1_4.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/iskenderkanimetov/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/iskenderkanimetov/Documents/univer-tasks/2025/first_semester/usupova_n_m/databases/excel_tasks/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{2E8AE0A0-55FF-9E45-88CE-F33C16D7B5D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E084150C-5B2C-FF41-99D9-E6D563788428}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="860" windowWidth="36000" windowHeight="22520" xr2:uid="{55021F89-182A-7043-91BF-296DAF14630F}"/>
+    <workbookView xWindow="0" yWindow="880" windowWidth="36000" windowHeight="21120" xr2:uid="{55021F89-182A-7043-91BF-296DAF14630F}"/>
   </bookViews>
   <sheets>
     <sheet name="График_1" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
     <definedName name="_xlchart.v1.2" hidden="1">График_1!$A$4:$A$84</definedName>
     <definedName name="_xlchart.v1.3" hidden="1">График_1!$B$4:$B$84</definedName>
   </definedNames>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -58,7 +58,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="0.0"/>
+    <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -122,13 +122,13 @@
   </cellStyleXfs>
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -163,8 +163,8 @@
     <c:autoTitleDeleted val="1"/>
     <c:plotArea>
       <c:layout/>
-      <c:lineChart>
-        <c:grouping val="standard"/>
+      <c:scatterChart>
+        <c:scatterStyle val="smoothMarker"/>
         <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
@@ -181,7 +181,7 @@
           <c:marker>
             <c:symbol val="none"/>
           </c:marker>
-          <c:cat>
+          <c:xVal>
             <c:numRef>
               <c:f>График_1!$A$4:$A$84</c:f>
               <c:numCache>
@@ -432,8 +432,8 @@
                 </c:pt>
               </c:numCache>
             </c:numRef>
-          </c:cat>
-          <c:val>
+          </c:xVal>
+          <c:yVal>
             <c:numRef>
               <c:f>График_1!$B$4:$B$84</c:f>
               <c:numCache>
@@ -684,8 +684,8 @@
                 </c:pt>
               </c:numCache>
             </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
+          </c:yVal>
+          <c:smooth val="1"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-D3D0-4642-A1D0-770B2E97678A}"/>
@@ -700,11 +700,10 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:smooth val="0"/>
         <c:axId val="1187869023"/>
         <c:axId val="1187684975"/>
-      </c:lineChart>
-      <c:catAx>
+      </c:scatterChart>
+      <c:valAx>
         <c:axId val="1187869023"/>
         <c:scaling>
           <c:orientation val="minMax"/>
@@ -750,11 +749,8 @@
         </c:txPr>
         <c:crossAx val="1187684975"/>
         <c:crosses val="autoZero"/>
-        <c:auto val="1"/>
-        <c:lblAlgn val="ctr"/>
-        <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="0"/>
-      </c:catAx>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
       <c:valAx>
         <c:axId val="1187684975"/>
         <c:scaling>
@@ -809,7 +805,7 @@
         </c:txPr>
         <c:crossAx val="1187869023"/>
         <c:crosses val="autoZero"/>
-        <c:crossBetween val="between"/>
+        <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:spPr>
         <a:noFill/>
@@ -1861,751 +1857,751 @@
   <dimension ref="A1:C84"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N6" sqref="N6"/>
+      <selection activeCell="I30" sqref="I30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
+      <c r="B1" s="3"/>
+      <c r="C1" s="3"/>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A3" s="2" t="s">
+      <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="1" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A4" s="3">
+      <c r="A4" s="2">
         <v>-4</v>
       </c>
-      <c r="B4" s="3">
+      <c r="B4" s="2">
         <f>5*SIN(A4)*COS(A4+1)</f>
         <v>-3.7461439588167145</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A5" s="3">
+      <c r="A5" s="2">
         <v>-3.9</v>
       </c>
-      <c r="B5" s="3">
+      <c r="B5" s="2">
         <f>5*SIN(A5)*COS(A5+1)</f>
         <v>-3.338960839866262</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A6" s="3">
+      <c r="A6" s="2">
         <v>-3.8</v>
       </c>
-      <c r="B6" s="3">
+      <c r="B6" s="2">
         <f t="shared" ref="B6:B69" si="0">5*SIN(A6)*COS(A6+1)</f>
         <v>-2.8825308708031856</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A7" s="3">
+      <c r="A7" s="2">
         <v>-3.7</v>
       </c>
-      <c r="B7" s="3">
+      <c r="B7" s="2">
         <f t="shared" si="0"/>
         <v>-2.3950504741459753</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A8" s="3">
+      <c r="A8" s="2">
         <v>-3.6</v>
       </c>
-      <c r="B8" s="3">
+      <c r="B8" s="2">
         <f t="shared" si="0"/>
         <v>-1.8959539549760005</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A9" s="3">
+      <c r="A9" s="2">
         <v>-3.5</v>
       </c>
-      <c r="B9" s="3">
+      <c r="B9" s="2">
         <f t="shared" si="0"/>
         <v>-1.4051387165224265</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A10" s="3">
+      <c r="A10" s="2">
         <v>-3.4</v>
       </c>
-      <c r="B10" s="3">
+      <c r="B10" s="2">
         <f t="shared" si="0"/>
         <v>-0.94217201348534785</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A11" s="3">
+      <c r="A11" s="2">
         <v>-3.3</v>
       </c>
-      <c r="B11" s="3">
+      <c r="B11" s="2">
         <f t="shared" si="0"/>
         <v>-0.52551086733893737</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A12" s="3">
+      <c r="A12" s="2">
         <v>-3.2</v>
       </c>
-      <c r="B12" s="3">
+      <c r="B12" s="2">
         <f t="shared" si="0"/>
         <v>-0.1717662431297734</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A13" s="3">
+      <c r="A13" s="2">
         <v>-3.1</v>
       </c>
-      <c r="B13" s="3">
+      <c r="B13" s="2">
         <f t="shared" si="0"/>
         <v>0.10495917728064171</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A14" s="3">
+      <c r="A14" s="2">
         <v>-3</v>
       </c>
-      <c r="B14" s="3">
+      <c r="B14" s="2">
         <f t="shared" si="0"/>
         <v>0.29363322463810493</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A15" s="3">
+      <c r="A15" s="2">
         <v>-2.9</v>
       </c>
-      <c r="B15" s="3">
+      <c r="B15" s="2">
         <f t="shared" si="0"/>
         <v>0.3867340600698605</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A16" s="3">
+      <c r="A16" s="2">
         <v>-2.8</v>
       </c>
-      <c r="B16" s="3">
+      <c r="B16" s="2">
         <f t="shared" si="0"/>
         <v>0.38055004706391982</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A17" s="3">
+      <c r="A17" s="2">
         <v>-2.7</v>
       </c>
-      <c r="B17" s="3">
+      <c r="B17" s="2">
         <f t="shared" si="0"/>
         <v>0.27532772270404893</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A18" s="3">
+      <c r="A18" s="2">
         <v>-2.6</v>
       </c>
-      <c r="B18" s="3">
+      <c r="B18" s="2">
         <f t="shared" si="0"/>
         <v>7.5261969014229102E-2</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A19" s="3">
+      <c r="A19" s="2">
         <v>-2.5</v>
       </c>
-      <c r="B19" s="3">
+      <c r="B19" s="2">
         <f t="shared" si="0"/>
         <v>-0.21167122374992062</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A20" s="3">
+      <c r="A20" s="2">
         <v>-2.4</v>
       </c>
-      <c r="B20" s="3">
+      <c r="B20" s="2">
         <f t="shared" si="0"/>
         <v>-0.57403273466294402</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A21" s="3">
+      <c r="A21" s="2">
         <v>-2.2999999999999998</v>
       </c>
-      <c r="B21" s="3">
+      <c r="B21" s="2">
         <f t="shared" si="0"/>
         <v>-0.99737635378261114</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A22" s="3">
+      <c r="A22" s="2">
         <v>-2.2000000000000002</v>
       </c>
-      <c r="B22" s="3">
+      <c r="B22" s="2">
         <f t="shared" si="0"/>
         <v>-1.4648247069526621</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A23" s="3">
+      <c r="A23" s="2">
         <v>-2.1</v>
       </c>
-      <c r="B23" s="3">
+      <c r="B23" s="2">
         <f t="shared" si="0"/>
         <v>-1.9577421034507911</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A24" s="3">
+      <c r="A24" s="2">
         <v>-2</v>
       </c>
-      <c r="B24" s="3">
+      <c r="B24" s="2">
         <f t="shared" si="0"/>
         <v>-2.4564774821694098</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A25" s="3">
+      <c r="A25" s="2">
         <v>-1.9</v>
       </c>
-      <c r="B25" s="3">
+      <c r="B25" s="2">
         <f t="shared" si="0"/>
         <v>-2.9411478374095035</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A26" s="3">
+      <c r="A26" s="2">
         <v>-1.8</v>
       </c>
-      <c r="B26" s="3">
+      <c r="B26" s="2">
         <f t="shared" si="0"/>
         <v>-3.3924308915734014</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A27" s="3">
+      <c r="A27" s="2">
         <v>-1.7</v>
       </c>
-      <c r="B27" s="3">
+      <c r="B27" s="2">
         <f t="shared" si="0"/>
         <v>-3.7923354133976188</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A28" s="3">
+      <c r="A28" s="2">
         <v>-1.6</v>
       </c>
-      <c r="B28" s="3">
+      <c r="B28" s="2">
         <f t="shared" si="0"/>
         <v>-4.1249184715687157</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A29" s="3">
+      <c r="A29" s="2">
         <v>-1.5</v>
       </c>
-      <c r="B29" s="3">
+      <c r="B29" s="2">
         <f t="shared" si="0"/>
         <v>-4.3769210290839462</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A30" s="3">
+      <c r="A30" s="2">
         <v>-1.4</v>
       </c>
-      <c r="B30" s="3">
+      <c r="B30" s="2">
         <f t="shared" si="0"/>
         <v>-4.5382965392152288</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A31" s="3">
+      <c r="A31" s="2">
         <v>-1.3</v>
       </c>
-      <c r="B31" s="3">
+      <c r="B31" s="2">
         <f t="shared" si="0"/>
         <v>-4.6026114696235041</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A32" s="3">
+      <c r="A32" s="2">
         <v>-1.2</v>
       </c>
-      <c r="B32" s="3">
+      <c r="B32" s="2">
         <f t="shared" si="0"/>
         <v>-4.5673017869908907</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A33" s="3">
+      <c r="A33" s="2">
         <v>-1.1000000000000001</v>
       </c>
-      <c r="B33" s="3">
+      <c r="B33" s="2">
         <f t="shared" si="0"/>
         <v>-4.4337751769378073</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A34" s="3">
+      <c r="A34" s="2">
         <v>-1</v>
       </c>
-      <c r="B34" s="3">
+      <c r="B34" s="2">
         <f t="shared" si="0"/>
         <v>-4.2073549240394827</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A35" s="3">
+      <c r="A35" s="2">
         <v>-0.9</v>
       </c>
-      <c r="B35" s="3">
+      <c r="B35" s="2">
         <f t="shared" si="0"/>
         <v>-3.8970676892685483</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A36" s="3">
+      <c r="A36" s="2">
         <v>-0.8</v>
       </c>
-      <c r="B36" s="3">
+      <c r="B36" s="2">
         <f t="shared" si="0"/>
         <v>-3.5152836455073295</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A37" s="3">
+      <c r="A37" s="2">
         <v>-0.7</v>
       </c>
-      <c r="B37" s="3">
+      <c r="B37" s="2">
         <f t="shared" si="0"/>
         <v>-3.077223317791367</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A38" s="3">
+      <c r="A38" s="2">
         <v>-0.6</v>
       </c>
-      <c r="B38" s="3">
+      <c r="B38" s="2">
         <f t="shared" si="0"/>
         <v>-2.6003507890073942</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A39" s="3">
+      <c r="A39" s="2">
         <v>-0.5</v>
       </c>
-      <c r="B39" s="3">
+      <c r="B39" s="2">
         <f t="shared" si="0"/>
         <v>-2.1036774620197414</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A40" s="3">
+      <c r="A40" s="2">
         <v>-0.4</v>
       </c>
-      <c r="B40" s="3">
+      <c r="B40" s="2">
         <f t="shared" si="0"/>
         <v>-1.6070041350320885</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A41" s="3">
+      <c r="A41" s="2">
         <v>-0.3</v>
       </c>
-      <c r="B41" s="3">
+      <c r="B41" s="2">
         <f t="shared" si="0"/>
         <v>-1.130131606248115</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A42" s="3">
+      <c r="A42" s="2">
         <v>-0.2</v>
       </c>
-      <c r="B42" s="3">
+      <c r="B42" s="2">
         <f t="shared" si="0"/>
         <v>-0.69207127853215289</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A43" s="3">
+      <c r="A43" s="2">
         <v>-0.1</v>
       </c>
-      <c r="B43" s="3">
+      <c r="B43" s="2">
         <f t="shared" si="0"/>
         <v>-0.31028723477093434</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A44" s="3">
+      <c r="A44" s="2">
         <v>0</v>
       </c>
-      <c r="B44" s="3">
+      <c r="B44" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A45" s="3">
+      <c r="A45" s="2">
         <v>9.9999999999999603E-2</v>
       </c>
-      <c r="B45" s="3">
+      <c r="B45" s="2">
         <f t="shared" si="0"/>
         <v>0.22642025289832388</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A46" s="3">
+      <c r="A46" s="2">
         <v>0.2</v>
       </c>
-      <c r="B46" s="3">
+      <c r="B46" s="2">
         <f t="shared" si="0"/>
         <v>0.35994686295140921</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A47" s="3">
+      <c r="A47" s="2">
         <v>0.3</v>
       </c>
-      <c r="B47" s="3">
+      <c r="B47" s="2">
         <f t="shared" si="0"/>
         <v>0.39525654558402151</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A48" s="3">
+      <c r="A48" s="2">
         <v>0.4</v>
       </c>
-      <c r="B48" s="3">
+      <c r="B48" s="2">
         <f t="shared" si="0"/>
         <v>0.33094161517574694</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A49" s="3">
+      <c r="A49" s="2">
         <v>0.5</v>
       </c>
-      <c r="B49" s="3">
+      <c r="B49" s="2">
         <f t="shared" si="0"/>
         <v>0.16956610504446296</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A50" s="3">
+      <c r="A50" s="2">
         <v>0.6</v>
       </c>
-      <c r="B50" s="3">
+      <c r="B50" s="2">
         <f t="shared" si="0"/>
         <v>-8.2436452470766058E-2</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A51" s="3">
+      <c r="A51" s="2">
         <v>0.7</v>
       </c>
-      <c r="B51" s="3">
+      <c r="B51" s="2">
         <f t="shared" si="0"/>
         <v>-0.41501951064186376</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A52" s="3">
+      <c r="A52" s="2">
         <v>0.8</v>
       </c>
-      <c r="B52" s="3">
+      <c r="B52" s="2">
         <f t="shared" si="0"/>
         <v>-0.81492403246608092</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A53" s="3">
+      <c r="A53" s="2">
         <v>0.9</v>
       </c>
-      <c r="B53" s="3">
+      <c r="B53" s="2">
         <f t="shared" si="0"/>
         <v>-1.2662070866299786</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A54" s="3">
+      <c r="A54" s="2">
         <v>1</v>
       </c>
-      <c r="B54" s="3">
+      <c r="B54" s="2">
         <f t="shared" si="0"/>
         <v>-1.7508774418700734</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A55" s="3">
+      <c r="A55" s="2">
         <v>1.1000000000000001</v>
       </c>
-      <c r="B55" s="3">
+      <c r="B55" s="2">
         <f t="shared" si="0"/>
         <v>-2.2496128205886916</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A56" s="3">
+      <c r="A56" s="2">
         <v>1.2</v>
       </c>
-      <c r="B56" s="3">
+      <c r="B56" s="2">
         <f t="shared" si="0"/>
         <v>-2.7425302170868195</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A57" s="3">
+      <c r="A57" s="2">
         <v>1.3</v>
       </c>
-      <c r="B57" s="3">
+      <c r="B57" s="2">
         <f t="shared" si="0"/>
         <v>-3.2099785702568719</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A58" s="3">
+      <c r="A58" s="2">
         <v>1.4</v>
       </c>
-      <c r="B58" s="3">
+      <c r="B58" s="2">
         <f t="shared" si="0"/>
         <v>-3.6333221893765382</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A59" s="3">
+      <c r="A59" s="2">
         <v>1.50000000000001</v>
       </c>
-      <c r="B59" s="3">
+      <c r="B59" s="2">
         <f t="shared" si="0"/>
         <v>-3.995683700289594</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A60" s="3">
+      <c r="A60" s="2">
         <v>1.6</v>
       </c>
-      <c r="B60" s="3">
+      <c r="B60" s="2">
         <f t="shared" si="0"/>
         <v>-4.2826168930537118</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A61" s="3">
+      <c r="A61" s="2">
         <v>1.7</v>
       </c>
-      <c r="B61" s="3">
+      <c r="B61" s="2">
         <f t="shared" si="0"/>
         <v>-4.4826826467435312</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A62" s="3">
+      <c r="A62" s="2">
         <v>1.80000000000001</v>
       </c>
-      <c r="B62" s="3">
+      <c r="B62" s="2">
         <f t="shared" si="0"/>
         <v>-4.5879049711034083</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A63" s="3">
+      <c r="A63" s="2">
         <v>1.9000000000000099</v>
       </c>
-      <c r="B63" s="3">
+      <c r="B63" s="2">
         <f t="shared" si="0"/>
         <v>-4.5940889841093391</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A64" s="3">
+      <c r="A64" s="2">
         <v>2.0000000000000102</v>
       </c>
-      <c r="B64" s="3">
+      <c r="B64" s="2">
         <f t="shared" si="0"/>
         <v>-4.5009881486775729</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A65" s="3">
+      <c r="A65" s="2">
         <v>2.1</v>
       </c>
-      <c r="B65" s="3">
+      <c r="B65" s="2">
         <f t="shared" si="0"/>
         <v>-4.3123141013201245</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A66" s="3">
+      <c r="A66" s="2">
         <v>2.2000000000000099</v>
       </c>
-      <c r="B66" s="3">
+      <c r="B66" s="2">
         <f t="shared" si="0"/>
         <v>-4.0355886809096777</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A67" s="3">
+      <c r="A67" s="2">
         <v>2.30000000000001</v>
       </c>
-      <c r="B67" s="3">
+      <c r="B67" s="2">
         <f t="shared" si="0"/>
         <v>-3.681844056700506</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A68" s="3">
+      <c r="A68" s="2">
         <v>2.4000000000000101</v>
       </c>
-      <c r="B68" s="3">
+      <c r="B68" s="2">
         <f t="shared" si="0"/>
         <v>-3.2651829105540897</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A69" s="3">
+      <c r="A69" s="2">
         <v>2.5000000000000102</v>
       </c>
-      <c r="B69" s="3">
+      <c r="B69" s="2">
         <f t="shared" si="0"/>
         <v>-2.8022162075170072</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A70" s="3">
+      <c r="A70" s="2">
         <v>2.6000000000000099</v>
       </c>
-      <c r="B70" s="3">
+      <c r="B70" s="2">
         <f t="shared" ref="B70:B84" si="1">5*SIN(A70)*COS(A70+1)</f>
         <v>-2.3114009690634338</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A71" s="3">
+      <c r="A71" s="2">
         <v>2.7000000000000099</v>
       </c>
-      <c r="B71" s="3">
+      <c r="B71" s="2">
         <f t="shared" si="1"/>
         <v>-1.8123044498934588</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A72" s="3">
+      <c r="A72" s="2">
         <v>2.80000000000001</v>
       </c>
-      <c r="B72" s="3">
+      <c r="B72" s="2">
         <f t="shared" si="1"/>
         <v>-1.3248240532362479</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A73" s="3">
+      <c r="A73" s="2">
         <v>2.9000000000000101</v>
       </c>
-      <c r="B73" s="3">
+      <c r="B73" s="2">
         <f t="shared" si="1"/>
         <v>-0.86839408417317643</v>
       </c>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A74" s="3">
+      <c r="A74" s="2">
         <v>3.0000000000000102</v>
       </c>
-      <c r="B74" s="3">
+      <c r="B74" s="2">
         <f t="shared" si="1"/>
         <v>-0.46121096522272981</v>
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A75" s="3">
+      <c r="A75" s="2">
         <v>3.1000000000000099</v>
       </c>
-      <c r="B75" s="3">
+      <c r="B75" s="2">
         <f t="shared" si="1"/>
         <v>-0.11950780239682858</v>
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A76" s="3">
+      <c r="A76" s="2">
         <v>3.2000000000000099</v>
       </c>
-      <c r="B76" s="3">
+      <c r="B76" s="2">
         <f t="shared" si="1"/>
         <v>0.14309277750934746</v>
       </c>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A77" s="3">
+      <c r="A77" s="2">
         <v>3.30000000000001</v>
       </c>
-      <c r="B77" s="3">
+      <c r="B77" s="2">
         <f t="shared" si="1"/>
         <v>0.3161217180589877</v>
       </c>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A78" s="3">
+      <c r="A78" s="2">
         <v>3.4000000000000101</v>
       </c>
-      <c r="B78" s="3">
+      <c r="B78" s="2">
         <f t="shared" si="1"/>
         <v>0.39268090141677386</v>
       </c>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A79" s="3">
+      <c r="A79" s="2">
         <v>3.5000000000000102</v>
       </c>
-      <c r="B79" s="3">
+      <c r="B79" s="2">
         <f t="shared" si="1"/>
         <v>0.36971815453870499</v>
       </c>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A80" s="3">
+      <c r="A80" s="2">
         <v>3.6000000000000099</v>
       </c>
-      <c r="B80" s="3">
+      <c r="B80" s="2">
         <f t="shared" si="1"/>
         <v>0.24814892967967328</v>
       </c>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A81" s="3">
+      <c r="A81" s="2">
         <v>3.7000000000000099</v>
       </c>
-      <c r="B81" s="3">
+      <c r="B81" s="2">
         <f t="shared" si="1"/>
         <v>3.281980820093456E-2</v>
       </c>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A82" s="3">
+      <c r="A82" s="2">
         <v>3.80000000000001</v>
       </c>
-      <c r="B82" s="3">
+      <c r="B82" s="2">
         <f t="shared" si="1"/>
         <v>-0.26768471733449112</v>
       </c>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A83" s="3">
+      <c r="A83" s="2">
         <v>3.9000000000000101</v>
       </c>
-      <c r="B83" s="3">
+      <c r="B83" s="2">
         <f t="shared" si="1"/>
         <v>-0.64138447979037683</v>
       </c>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A84" s="3">
+      <c r="A84" s="2">
         <v>4.0000000000000098</v>
       </c>
-      <c r="B84" s="3">
+      <c r="B84" s="2">
         <f t="shared" si="1"/>
         <v>-1.0733812489153944</v>
       </c>

</xml_diff>